<commit_message>
Turicreate models and basic interface build
</commit_message>
<xml_diff>
--- a/config/ranking_methodology.xlsx
+++ b/config/ranking_methodology.xlsx
@@ -130,10 +130,10 @@
     <t xml:space="preserve">2019 NIH specialty funding</t>
   </si>
   <si>
+    <t xml:space="preserve">Teaching quality</t>
+  </si>
+  <si>
     <t xml:space="preserve">Program setting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teaching quality</t>
   </si>
   <si>
     <t xml:space="preserve">Family medicine board pass rate</t>
@@ -267,15 +267,16 @@
   </sheetPr>
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,13 +304,14 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>0.3</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A2)</f>
+        <v>0.4</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>8</v>
@@ -323,7 +325,8 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0.3</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A3)</f>
+        <v>0.4</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>10</v>
@@ -343,7 +346,8 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.3</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A4)</f>
+        <v>0.4</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
@@ -363,7 +367,8 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0.3</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A5)</f>
+        <v>0.4</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>12</v>
@@ -383,7 +388,8 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.3</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A6)</f>
+        <v>0.4</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>13</v>
@@ -403,13 +409,14 @@
         <v>14</v>
       </c>
       <c r="B7" s="1" t="n">
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A7)</f>
         <v>0.1</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>8</v>
@@ -423,13 +430,14 @@
         <v>14</v>
       </c>
       <c r="B8" s="1" t="n">
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A8)</f>
         <v>0.1</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0.025</v>
+        <v>0.02</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>8</v>
@@ -443,13 +451,14 @@
         <v>14</v>
       </c>
       <c r="B9" s="1" t="n">
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A9)</f>
         <v>0.1</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>0.025</v>
+        <v>0.02</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>8</v>
@@ -463,13 +472,14 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A10)</f>
+        <v>0.1</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>8</v>
@@ -483,7 +493,8 @@
         <v>18</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A11)</f>
+        <v>0.1</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>20</v>
@@ -503,7 +514,8 @@
         <v>18</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A12)</f>
+        <v>0.1</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>22</v>
@@ -523,14 +535,13 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A13)</f>
+        <v>0</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="1" t="n">
-        <v>0.05</v>
-      </c>
+      <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
@@ -543,15 +554,13 @@
         <v>23</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A14)</f>
+        <v>0</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="1" t="n">
-        <f aca="false">0.1/6</f>
-        <v>0.0166666666666667</v>
-      </c>
+      <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
@@ -564,15 +573,13 @@
         <v>23</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A15)</f>
+        <v>0</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="1" t="n">
-        <f aca="false">0.1/6</f>
-        <v>0.0166666666666667</v>
-      </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="1" t="s">
         <v>25</v>
       </c>
@@ -585,15 +592,13 @@
         <v>23</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A16)</f>
+        <v>0</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="1" t="n">
-        <f aca="false">0.1/6</f>
-        <v>0.0166666666666667</v>
-      </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
@@ -606,15 +611,13 @@
         <v>23</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A17)</f>
+        <v>0</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="1" t="n">
-        <f aca="false">0.1/6</f>
-        <v>0.0166666666666667</v>
-      </c>
+      <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
         <v>25</v>
       </c>
@@ -627,15 +630,13 @@
         <v>23</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A18)</f>
+        <v>0</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="1" t="n">
-        <f aca="false">0.1/6</f>
-        <v>0.0166666666666667</v>
-      </c>
+      <c r="D18" s="1"/>
       <c r="E18" s="1" t="s">
         <v>25</v>
       </c>
@@ -648,15 +649,13 @@
         <v>23</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A19)</f>
+        <v>0</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="1" t="n">
-        <f aca="false">0.1/6</f>
-        <v>0.0166666666666667</v>
-      </c>
+      <c r="D19" s="1"/>
       <c r="E19" s="1" t="s">
         <v>25</v>
       </c>
@@ -669,13 +668,14 @@
         <v>32</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A20)</f>
+        <v>0.17</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>34</v>
@@ -689,7 +689,8 @@
         <v>32</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A21)</f>
+        <v>0.17</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>35</v>
@@ -706,16 +707,17 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A22)</f>
+        <v>0.3</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>8</v>
@@ -726,16 +728,17 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A23)</f>
+        <v>0.3</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>38</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>0.025</v>
+        <v>0.01</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>39</v>
@@ -746,16 +749,17 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A24)</f>
+        <v>0.3</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>0.025</v>
+        <v>0.01</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>41</v>
@@ -766,16 +770,17 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A25)</f>
+        <v>0.3</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>42</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>0.025</v>
+        <v>0.01</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>43</v>
@@ -786,16 +791,17 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A26)</f>
+        <v>0.3</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>44</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>0.025</v>
+        <v>0.01</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>45</v>
@@ -806,16 +812,17 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>0.15</v>
+        <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A27)</f>
+        <v>0.3</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>46</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
build recommendation and filtering UI
</commit_message>
<xml_diff>
--- a/config/ranking_methodology.xlsx
+++ b/config/ranking_methodology.xlsx
@@ -268,10 +268,10 @@
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="155" zoomScaleNormal="155" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.59"/>
@@ -473,13 +473,13 @@
       </c>
       <c r="B10" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A10)</f>
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>8</v>
@@ -494,13 +494,13 @@
       </c>
       <c r="B11" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A11)</f>
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>8</v>
@@ -515,13 +515,13 @@
       </c>
       <c r="B12" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A12)</f>
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>8</v>
@@ -536,12 +536,14 @@
       </c>
       <c r="B13" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A13)</f>
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="n">
+        <v>0.05</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
@@ -555,12 +557,14 @@
       </c>
       <c r="B14" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A14)</f>
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="n">
+        <v>0.01</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
@@ -574,12 +578,14 @@
       </c>
       <c r="B15" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A15)</f>
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="n">
+        <v>0.01</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>25</v>
       </c>
@@ -593,12 +599,14 @@
       </c>
       <c r="B16" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A16)</f>
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1" t="n">
+        <v>0.01</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
@@ -612,12 +620,14 @@
       </c>
       <c r="B17" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A17)</f>
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="n">
+        <v>0.01</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>25</v>
       </c>
@@ -631,12 +641,14 @@
       </c>
       <c r="B18" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A18)</f>
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1" t="n">
+        <v>0.01</v>
+      </c>
       <c r="E18" s="1" t="s">
         <v>25</v>
       </c>
@@ -650,12 +662,14 @@
       </c>
       <c r="B19" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A19)</f>
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1" t="n">
+        <v>0.01</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>25</v>
       </c>
@@ -711,13 +725,13 @@
       </c>
       <c r="B22" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A22)</f>
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>37</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>8</v>
@@ -732,7 +746,7 @@
       </c>
       <c r="B23" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A23)</f>
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>38</v>
@@ -753,7 +767,7 @@
       </c>
       <c r="B24" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A24)</f>
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>40</v>
@@ -774,7 +788,7 @@
       </c>
       <c r="B25" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A25)</f>
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>42</v>
@@ -795,7 +809,7 @@
       </c>
       <c r="B26" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A26)</f>
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>44</v>
@@ -816,7 +830,7 @@
       </c>
       <c r="B27" s="1" t="n">
         <f aca="false">SUMIFS($D$2:$D$27,$A$2:$A$27,$A27)</f>
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>46</v>

</xml_diff>